<commit_message>
Added variable for direction of indicators (positive, negative, no direction)
</commit_message>
<xml_diff>
--- a/DS-D files/Key messages.xlsx
+++ b/DS-D files/Key messages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5fa83f01ffb69574/R/DDI/DS-D files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{115FF2DC-93EB-4FBD-B2A8-C0CC45B7190F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EC8B6DA-9A2D-4EF8-82AD-46E9DB1569A9}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="8_{115FF2DC-93EB-4FBD-B2A8-C0CC45B7190F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65EB6137-568B-438E-8A2D-430B303230A4}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="15" windowWidth="28455" windowHeight="16185" xr2:uid="{DF5D2554-F1D8-4083-8A6A-01334C00ED3B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{DF5D2554-F1D8-4083-8A6A-01334C00ED3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="112">
   <si>
     <t xml:space="preserve">The proportion of adults with disabilities varies across countries, with the lowest at 5%, the highest at 33%, and the median at 14.2%. </t>
   </si>
@@ -609,6 +609,9 @@
   </si>
   <si>
     <t>IndicatorName</t>
+  </si>
+  <si>
+    <t>Direction</t>
   </si>
 </sst>
 </file>
@@ -1017,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F80B718-1375-4CF0-862D-AA7D94D95BA4}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1030,7 +1033,7 @@
     <col min="3" max="3" width="33.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>104</v>
       </c>
@@ -1046,8 +1049,11 @@
       <c r="E1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>105</v>
       </c>
@@ -1064,7 +1070,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -1081,7 +1087,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>106</v>
       </c>
@@ -1097,8 +1103,11 @@
       <c r="E4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>106</v>
       </c>
@@ -1114,8 +1123,11 @@
       <c r="E5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>106</v>
       </c>
@@ -1131,8 +1143,11 @@
       <c r="E6" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>106</v>
       </c>
@@ -1148,8 +1163,11 @@
       <c r="E7" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>107</v>
       </c>
@@ -1165,8 +1183,11 @@
       <c r="E8" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>107</v>
       </c>
@@ -1182,8 +1203,11 @@
       <c r="E9" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>107</v>
       </c>
@@ -1199,8 +1223,11 @@
       <c r="E10" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>107</v>
       </c>
@@ -1216,8 +1243,11 @@
       <c r="E11" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>108</v>
       </c>
@@ -1233,8 +1263,11 @@
       <c r="E12" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>108</v>
       </c>
@@ -1250,8 +1283,11 @@
       <c r="E13" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>108</v>
       </c>
@@ -1267,8 +1303,11 @@
       <c r="E14" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>108</v>
       </c>
@@ -1284,8 +1323,11 @@
       <c r="E15" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>108</v>
       </c>
@@ -1301,8 +1343,11 @@
       <c r="E16" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>108</v>
       </c>
@@ -1318,8 +1363,11 @@
       <c r="E17" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>108</v>
       </c>
@@ -1335,8 +1383,11 @@
       <c r="E18" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>108</v>
       </c>
@@ -1353,7 +1404,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>109</v>
       </c>
@@ -1369,8 +1420,11 @@
       <c r="E20" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>109</v>
       </c>
@@ -1386,8 +1440,11 @@
       <c r="E21" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>109</v>
       </c>
@@ -1403,8 +1460,11 @@
       <c r="E22" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>109</v>
       </c>
@@ -1420,8 +1480,11 @@
       <c r="E23" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>109</v>
       </c>
@@ -1437,8 +1500,11 @@
       <c r="E24" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>109</v>
       </c>
@@ -1454,8 +1520,11 @@
       <c r="E25" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>109</v>
       </c>
@@ -1472,7 +1541,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>109</v>
       </c>
@@ -1488,8 +1557,11 @@
       <c r="E27" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>109</v>
       </c>
@@ -1505,8 +1577,11 @@
       <c r="E28" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>109</v>
       </c>
@@ -1522,8 +1597,11 @@
       <c r="E29" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -1538,6 +1616,9 @@
       </c>
       <c r="E30" t="s">
         <v>71</v>
+      </c>
+      <c r="F30" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update direction of indicators based on feedback
</commit_message>
<xml_diff>
--- a/DS-D files/Key messages.xlsx
+++ b/DS-D files/Key messages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5fa83f01ffb69574/R/DDI/DS-D files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="8_{115FF2DC-93EB-4FBD-B2A8-C0CC45B7190F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65EB6137-568B-438E-8A2D-430B303230A4}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="8_{115FF2DC-93EB-4FBD-B2A8-C0CC45B7190F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39849E37-FF75-4251-90FF-86135970547D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{DF5D2554-F1D8-4083-8A6A-01334C00ED3B}"/>
+    <workbookView xWindow="345" yWindow="15" windowWidth="28455" windowHeight="16185" xr2:uid="{DF5D2554-F1D8-4083-8A6A-01334C00ED3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1023,7 +1023,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1597,9 +1597,6 @@
       <c r="E29" t="s">
         <v>70</v>
       </c>
-      <c r="F29" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">

</xml_diff>

<commit_message>
Addition of insecurity indicator group
</commit_message>
<xml_diff>
--- a/DS-D files/Key messages.xlsx
+++ b/DS-D files/Key messages.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5fa83f01ffb69574/R/DDI/DS-D files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="8_{115FF2DC-93EB-4FBD-B2A8-C0CC45B7190F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39849E37-FF75-4251-90FF-86135970547D}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="8_{115FF2DC-93EB-4FBD-B2A8-C0CC45B7190F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFB4E9F2-0B8E-4C46-A004-2151F482026A}"/>
   <bookViews>
     <workbookView xWindow="345" yWindow="15" windowWidth="28455" windowHeight="16185" xr2:uid="{DF5D2554-F1D8-4083-8A6A-01334C00ED3B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="113">
   <si>
     <t xml:space="preserve">The proportion of adults with disabilities varies across countries, with the lowest at 5%, the highest at 33%, and the median at 14.2%. </t>
   </si>
@@ -612,6 +612,9 @@
   </si>
   <si>
     <t>Direction</t>
+  </si>
+  <si>
+    <t>Insecurity</t>
   </si>
 </sst>
 </file>
@@ -1023,7 +1026,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1506,7 +1509,7 @@
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B25" t="s">
         <v>44</v>
@@ -1526,7 +1529,7 @@
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B26" t="s">
         <v>46</v>
@@ -1543,7 +1546,7 @@
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B27" t="s">
         <v>48</v>
@@ -1563,7 +1566,7 @@
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B28" t="s">
         <v>50</v>
@@ -1583,7 +1586,7 @@
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B29" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Added colour selector and classified indicators according to directionality.
</commit_message>
<xml_diff>
--- a/DS-D files/Key messages.xlsx
+++ b/DS-D files/Key messages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5fa83f01ffb69574/R/DDI/DS-D files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5FA83F01FFB69574/R/DDI/DS-D files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="77" documentId="8_{115FF2DC-93EB-4FBD-B2A8-C0CC45B7190F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFB4E9F2-0B8E-4C46-A004-2151F482026A}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="15" windowWidth="28455" windowHeight="16185" xr2:uid="{DF5D2554-F1D8-4083-8A6A-01334C00ED3B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{DF5D2554-F1D8-4083-8A6A-01334C00ED3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1026,7 +1026,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>